<commit_message>
parse Stuller Classic Bands Mens5
</commit_message>
<xml_diff>
--- a/Stuller Classic Bands.xlsx
+++ b/Stuller Classic Bands.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Desktop\WEBSITE CONTENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\J\canary.webremote.net\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="72">
   <si>
     <t>Model</t>
   </si>
@@ -101,33 +101,12 @@
     <t>18k Rose Gold</t>
   </si>
   <si>
-    <t>BHRL72M14W</t>
-  </si>
-  <si>
     <t>Stuller</t>
   </si>
   <si>
     <t>Classic</t>
   </si>
   <si>
-    <t>BHRL72M14Y</t>
-  </si>
-  <si>
-    <t>BHRL72M14R</t>
-  </si>
-  <si>
-    <t>BHRL72M18W</t>
-  </si>
-  <si>
-    <t>BHRL72M18Y</t>
-  </si>
-  <si>
-    <t>BHRL72MPT</t>
-  </si>
-  <si>
-    <t>BHRL72MPAL</t>
-  </si>
-  <si>
     <t xml:space="preserve">platinum </t>
   </si>
   <si>
@@ -140,81 +119,12 @@
     <t>bands,wedding bands,anniversary bands,eternity bands,plain bands,diamond bands,diamond,diamonds ,loose diamonds,engagement ring,proposal,wedding rings,jewelry,fine jewelry,diamond jewelry,diamond rings,18k gold,gold,14k gold,platinum,sterling silver,silver,pearls,sapphire,emerald,ruby,earrings,necklaces,bracelets,rings,diamond education,guidance,diamonds and fine jewelry,ideal cut,excellent cut,GIA,AGS,IGI,cut,clarity,color,carat,settings,engaged</t>
   </si>
   <si>
-    <t>BHRL725M14W</t>
-  </si>
-  <si>
-    <t>BHRL725M14Y</t>
-  </si>
-  <si>
-    <t>BHRL725M14R</t>
-  </si>
-  <si>
-    <t>BHRL725M18W</t>
-  </si>
-  <si>
-    <t>BHRL725M18Y</t>
-  </si>
-  <si>
-    <t>BHRL725MPT</t>
-  </si>
-  <si>
-    <t>BHRL725MPAL</t>
-  </si>
-  <si>
     <t>2.5mm</t>
   </si>
   <si>
-    <t>BHRL725M18R</t>
-  </si>
-  <si>
-    <t>BHRL73M14W</t>
-  </si>
-  <si>
-    <t>BHRL73M14Y</t>
-  </si>
-  <si>
-    <t>BHRL73M14R</t>
-  </si>
-  <si>
-    <t>BHRL73M18W</t>
-  </si>
-  <si>
-    <t>BHRL73M18Y</t>
-  </si>
-  <si>
-    <t>BHRL73M18R</t>
-  </si>
-  <si>
-    <t>BHRL73MPT</t>
-  </si>
-  <si>
-    <t>BHRL73MPAL</t>
-  </si>
-  <si>
     <t>3mm</t>
   </si>
   <si>
-    <t>BHRL74M14W</t>
-  </si>
-  <si>
-    <t>BHRL74M14Y</t>
-  </si>
-  <si>
-    <t>BHRL74M14R</t>
-  </si>
-  <si>
-    <t>BHRL74M18W</t>
-  </si>
-  <si>
-    <t>BHRL74M18Y</t>
-  </si>
-  <si>
-    <t>BHRL74MPT</t>
-  </si>
-  <si>
-    <t>BHRL74MPAL</t>
-  </si>
-  <si>
     <t>4mm</t>
   </si>
   <si>
@@ -318,12 +228,24 @@
   </si>
   <si>
     <t>14K White Gold 2mm Classic Wedding Ring</t>
+  </si>
+  <si>
+    <t>BHRL72M</t>
+  </si>
+  <si>
+    <t>BHRL725M</t>
+  </si>
+  <si>
+    <t>BHRL73M</t>
+  </si>
+  <si>
+    <t>BHRL74M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,7 +333,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -726,9 +648,9 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="40.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -809,37 +731,37 @@
     </row>
     <row r="2" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S2" s="1">
         <v>120</v>
@@ -847,37 +769,37 @@
     </row>
     <row r="3" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S3" s="1">
         <v>120</v>
@@ -885,37 +807,37 @@
     </row>
     <row r="4" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S4" s="1">
         <v>130</v>
@@ -923,37 +845,37 @@
     </row>
     <row r="5" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S5" s="1">
         <v>170</v>
@@ -961,37 +883,37 @@
     </row>
     <row r="6" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S6" s="1">
         <v>170</v>
@@ -999,37 +921,37 @@
     </row>
     <row r="7" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S7" s="1">
         <v>220</v>
@@ -1037,37 +959,37 @@
     </row>
     <row r="8" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S8" s="1">
         <v>115</v>
@@ -1075,37 +997,37 @@
     </row>
     <row r="9" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S9" s="1">
         <v>135</v>
@@ -1113,37 +1035,37 @@
     </row>
     <row r="10" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S10" s="1">
         <v>135</v>
@@ -1151,37 +1073,37 @@
     </row>
     <row r="11" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S11" s="1">
         <v>135</v>
@@ -1189,37 +1111,37 @@
     </row>
     <row r="12" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S12" s="1">
         <v>195</v>
@@ -1227,37 +1149,37 @@
     </row>
     <row r="13" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S13" s="1">
         <v>195</v>
@@ -1265,37 +1187,37 @@
     </row>
     <row r="14" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S14" s="1">
         <v>195</v>
@@ -1303,37 +1225,37 @@
     </row>
     <row r="15" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S15" s="1">
         <v>300</v>
@@ -1341,37 +1263,37 @@
     </row>
     <row r="16" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S16" s="1">
         <v>130</v>
@@ -1379,37 +1301,37 @@
     </row>
     <row r="17" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S17" s="1">
         <v>165</v>
@@ -1417,37 +1339,37 @@
     </row>
     <row r="18" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S18" s="1">
         <v>165</v>
@@ -1455,37 +1377,37 @@
     </row>
     <row r="19" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S19" s="1">
         <v>165</v>
@@ -1493,37 +1415,37 @@
     </row>
     <row r="20" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S20" s="1">
         <v>225</v>
@@ -1531,37 +1453,37 @@
     </row>
     <row r="21" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S21" s="1">
         <v>225</v>
@@ -1569,37 +1491,37 @@
     </row>
     <row r="22" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S22" s="1">
         <v>225</v>
@@ -1607,37 +1529,37 @@
     </row>
     <row r="23" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S23" s="1">
         <v>350</v>
@@ -1645,37 +1567,37 @@
     </row>
     <row r="24" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S24" s="1">
         <v>160</v>
@@ -1683,37 +1605,37 @@
     </row>
     <row r="25" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S25" s="1">
         <v>210</v>
@@ -1721,37 +1643,37 @@
     </row>
     <row r="26" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S26" s="1">
         <v>210</v>
@@ -1759,37 +1681,37 @@
     </row>
     <row r="27" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S27" s="1">
         <v>210</v>
@@ -1797,37 +1719,37 @@
     </row>
     <row r="28" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S28" s="1">
         <v>270</v>
@@ -1835,37 +1757,37 @@
     </row>
     <row r="29" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S29" s="1">
         <v>270</v>
@@ -1873,37 +1795,37 @@
     </row>
     <row r="30" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S30" s="1">
         <v>470</v>
@@ -1911,37 +1833,37 @@
     </row>
     <row r="31" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S31" s="1">
         <v>200</v>

</xml_diff>